<commit_message>
updated fields and searching
</commit_message>
<xml_diff>
--- a/www/MouseSampleTemplate.xlsx
+++ b/www/MouseSampleTemplate.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">MOUSE STRAIN</t>
   </si>
   <si>
+    <t xml:space="preserve">MOUSE STRAIN GENOTYPE</t>
+  </si>
+  <si>
     <t xml:space="preserve">DOB</t>
   </si>
   <si>
@@ -53,7 +56,7 @@
     <t xml:space="preserve">DECAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Formulation(FT or Vehicle)</t>
+    <t xml:space="preserve">Formulation(FT, Vehicle, or None)</t>
   </si>
   <si>
     <t xml:space="preserve">Animal #</t>
@@ -65,6 +68,9 @@
     <t xml:space="preserve">CBA/CAJ</t>
   </si>
   <si>
+    <t xml:space="preserve">wild-type </t>
+  </si>
+  <si>
     <t xml:space="preserve">110dB_2hrs_3days</t>
   </si>
   <si>
@@ -83,9 +89,27 @@
     <t xml:space="preserve">#Controlled vocabulary. Do not edit!</t>
   </si>
   <si>
+    <t xml:space="preserve">Strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype</t>
+  </si>
+  <si>
     <t xml:space="preserve">Deafing Method</t>
   </si>
   <si>
+    <t xml:space="preserve">Fixation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestin,DTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestin +/-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Male</t>
   </si>
   <si>
@@ -95,16 +119,46 @@
     <t xml:space="preserve">WASHU</t>
   </si>
   <si>
+    <t xml:space="preserve">DTA+/+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Female</t>
   </si>
   <si>
+    <t xml:space="preserve">Creighton University ARF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2% PFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14% EDTA</t>
+  </si>
+  <si>
     <t xml:space="preserve">110dB_8hrs_5days</t>
   </si>
   <si>
+    <t xml:space="preserve">Avastus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTA-/-</t>
+  </si>
+  <si>
     <t xml:space="preserve">113dB_8hrs_5days</t>
   </si>
   <si>
+    <t xml:space="preserve">8 mg/kg CDX s.c.; (8wks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestin +/-, DTA+/+</t>
+  </si>
+  <si>
     <t xml:space="preserve">8 mg/kg_CDX_s.c._9.5 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestin +/-, DTA-/-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.225mg/g Tamoxifen, IP injection</t>
   </si>
 </sst>
 </file>
@@ -202,7 +256,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,20 +293,32 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -332,34 +398,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U109"/>
+  <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="1" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="17" style="0" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="1" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="18" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="1" width="28.99"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="D1" s="3"/>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -381,15 +447,18 @@
       <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="L1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="6"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -428,57 +497,63 @@
       <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="M2" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="9" t="n">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="n">
         <v>43832</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="E3" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="H3" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="J3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="5" t="n">
         <v>1622</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="6"/>
-      <c r="Q3" s="6"/>
+      <c r="M3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="10"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -487,33 +562,53 @@
     <row r="54" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="108" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
     </row>
     <row r="109" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B3:B1003" type="date">
+  <dataValidations count="11">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C1003" type="date">
       <formula1>43466</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D1003 F3:G1003" type="decimal">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E1003 G3:H1003" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C1003" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D1003" type="list">
       <formula1>Vocab!$C$4:$C$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E1003" type="list">
-      <formula1>Vocab!$E$4:$E$8</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L3:L1003" type="list">
-      <formula1>Vocab!$K$4:$K$5</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L1:L2" type="none">
-      <formula1>Vocab!$K$4:$K$5</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M3:M1003" type="list">
+      <formula1>Vocab!$K$4:$K$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M1:M2" type="none">
+      <formula1>Vocab!$K$4:$K$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1 J3:J1003" type="list">
+      <formula1>Vocab!$Q$4:$Q$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F3:F1003" type="list">
+      <formula1>Vocab!$E$4:$E$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I3:I1003" type="list">
+      <formula1>Vocab!$O$4:$O$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A1003" type="list">
+      <formula1>Vocab!$A$4:$A$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B1003" type="list">
+      <formula1>Vocab!$B$4:$B$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B2" type="none">
+      <formula1>Vocab!$B$4:$B$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -532,74 +627,142 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="1" sqref="A1:L1 K7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="12" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="12" t="s">
-        <v>27</v>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="d9d0" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>